<commit_message>
To Update some Annotations
</commit_message>
<xml_diff>
--- a/Infopine_SpringBoot_Assignment_V1.0_24Dec2020.xlsx
+++ b/Infopine_SpringBoot_Assignment_V1.0_24Dec2020.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="VersionControl" sheetId="6" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="General" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Index!$C$5:$I$97</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Index!$C$5:$I$99</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Spring!$A$1:$F$40</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="208">
   <si>
     <t>Subject</t>
   </si>
@@ -3949,9 +3949,6 @@
     <t>https://cloud.google.com/solutions/using-clusters-for-large-scale-technical-computing#:~:text=Google%20Cloud%20provides%20project-level,versions%2C%20or%20sync%20cluster%20configurations.</t>
   </si>
   <si>
-    <t>Google Cloud provides project-level identity and access management tools to allow controlled access to data and analytic tools. Authorized users can access the same apps, data, and clusters to ensure that everyone is on the same page without having to copy data, manage versions, or sync cluster configurations.</t>
-  </si>
-  <si>
     <t>What is GC and how does it help distributed computing?</t>
   </si>
   <si>
@@ -4864,12 +4861,58 @@
 A fork is a copy of a repository that allows you to freely experiment with changes without affecting the original project.
 The fork acts as a bridge between the original repository and (local/requester) personal copy where can contribute back to the original project using Pull Requests.</t>
   </si>
+  <si>
+    <t xml:space="preserve"> @Inject</t>
+  </si>
+  <si>
+    <t>Google Cloud provides project-level identity and access management tools to allow controlled access to data and analytic tools. 
+Authorized users can access the same apps, data, and clusters to ensure that everyone is on the same page without having to copy data, manage versions, or sync cluster configurations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @Resource</t>
+  </si>
+  <si>
+    <t>Completed - 18-01-2021</t>
+  </si>
+  <si>
+    <t>This annotation provide classes with a declarative way to resolve.
+  Its belongs to "org.springframework.beans.factory.annotation".
+  It can resolve dependencies either by field injection or by setter injection.
+  It allows you to mark it as non-mandatory.
+It supports below execution paths: 
+ Matches by Type
+ Restricts by Qualifiers
+ Matches by Name</t>
+  </si>
+  <si>
+    <t>This annotation provide classes with a declarative way to resolve.
+Its belongs to "javax.annotation.Resource"
+It can resolve dependencies either by field injection or by setter injection
+It allows you to specify a name of the injected bean
+Its part of the JSR250, and it supports below execution paths: 
+  Match by Name
+  Match by Type
+  Match by Qualifier / Restricts by Qualifiers (ignored if match is found by name)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @Autowired</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @Lazy</t>
+  </si>
+  <si>
+    <t>Annotation based on JSR-330
+It supports below execution paths: 
+ Matches by Type
+ Restricts by Qualifiers
+ Matches by Name</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5027,6 +5070,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -5183,7 +5232,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -5416,9 +5465,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -5427,6 +5473,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6661,8 +6719,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B5:K97" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" tableBorderDxfId="33">
-  <autoFilter ref="B5:K97"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B5:K99" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34" tableBorderDxfId="33">
+  <autoFilter ref="B5:K99"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Sr.No" dataDxfId="32"/>
     <tableColumn id="2" name="Subject" dataDxfId="31" dataCellStyle="Hyperlink"/>
@@ -6680,7 +6738,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B5:D44" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="B5:D46" totalsRowShown="0" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19">
   <tableColumns count="3">
     <tableColumn id="1" name="Sr.No." dataDxfId="18"/>
     <tableColumn id="2" name="Questions / Assignments" dataDxfId="17"/>
@@ -7067,11 +7125,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K97"/>
+  <dimension ref="A1:K99"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7280,7 +7338,7 @@
         <v>58</v>
       </c>
       <c r="D12" s="41" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>8</v>
@@ -7317,10 +7375,10 @@
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="J13" s="68" t="s">
         <v>193</v>
-      </c>
-      <c r="J13" s="68" t="s">
-        <v>194</v>
       </c>
       <c r="K13" s="7"/>
     </row>
@@ -7343,10 +7401,10 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J14" s="68" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K14" s="7"/>
     </row>
@@ -7591,7 +7649,7 @@
       <c r="C25" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="41" t="s">
         <v>75</v>
       </c>
       <c r="E25" s="1" t="s">
@@ -7602,7 +7660,9 @@
         <v>9</v>
       </c>
       <c r="H25" s="1"/>
-      <c r="I25" s="7"/>
+      <c r="I25" s="21" t="s">
+        <v>202</v>
+      </c>
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
     </row>
@@ -7635,7 +7695,7 @@
       <c r="C27" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="22" t="s">
+      <c r="D27" s="41" t="s">
         <v>77</v>
       </c>
       <c r="E27" s="1" t="s">
@@ -7646,7 +7706,9 @@
         <v>9</v>
       </c>
       <c r="H27" s="1"/>
-      <c r="I27" s="7"/>
+      <c r="I27" s="21" t="s">
+        <v>202</v>
+      </c>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
     </row>
@@ -9243,6 +9305,38 @@
         <v>185</v>
       </c>
       <c r="K97" s="7"/>
+    </row>
+    <row r="98" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B98" s="24">
+        <v>93</v>
+      </c>
+      <c r="C98" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="D98" s="57" t="s">
+        <v>199</v>
+      </c>
+      <c r="E98" s="18"/>
+      <c r="F98" s="18"/>
+      <c r="G98" s="19"/>
+      <c r="H98" s="18"/>
+      <c r="I98" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="J98" s="86"/>
+      <c r="K98" s="72"/>
+    </row>
+    <row r="99" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B99" s="24"/>
+      <c r="C99" s="84"/>
+      <c r="D99" s="72"/>
+      <c r="E99" s="18"/>
+      <c r="F99" s="18"/>
+      <c r="G99" s="19"/>
+      <c r="H99" s="18"/>
+      <c r="I99" s="85"/>
+      <c r="J99" s="86"/>
+      <c r="K99" s="72"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -9297,6 +9391,9 @@
     <hyperlink ref="D13" location="General!C10" display="What do you know about GCP?"/>
     <hyperlink ref="D14" location="General!C11" display="How do Kubernetes sit on GC ?"/>
     <hyperlink ref="J14" r:id="rId9"/>
+    <hyperlink ref="D25" location="Spring!C10" display="@Resource"/>
+    <hyperlink ref="D27" location="Spring!C12" display="@Autowired"/>
+    <hyperlink ref="D98" location="Spring!C45" display=" @Inject"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>
@@ -9309,11 +9406,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9326,18 +9423,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="83" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="80"/>
+      <c r="A2" s="83"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="80"/>
+      <c r="A3" s="83"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="80"/>
+      <c r="A4" s="83"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
@@ -9397,15 +9494,17 @@
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="25">
         <v>5</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" s="5"/>
+        <v>201</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
@@ -9413,18 +9512,20 @@
         <v>6</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="25">
         <v>7</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" s="5"/>
+        <v>205</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
@@ -9724,13 +9825,31 @@
       </c>
     </row>
     <row r="44" spans="2:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="B44" s="16"/>
+      <c r="B44" s="16">
+        <v>39</v>
+      </c>
       <c r="C44" s="16" t="s">
         <v>173</v>
       </c>
       <c r="D44" s="62" t="s">
         <v>174</v>
       </c>
+    </row>
+    <row r="45" spans="2:4" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="16">
+        <v>40</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="D45" s="62" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -9753,8 +9872,8 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <pane ySplit="5" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9767,7 +9886,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="83" t="s">
         <v>110</v>
       </c>
       <c r="B1" s="4"/>
@@ -9776,21 +9895,21 @@
       <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="80"/>
+      <c r="A2" s="83"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="80"/>
+      <c r="A3" s="83"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="80"/>
+      <c r="A4" s="83"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -9938,7 +10057,7 @@
         <v>74</v>
       </c>
       <c r="E14" s="43" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="114.75" x14ac:dyDescent="0.25">
@@ -10073,9 +10192,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10087,7 +10206,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="83" t="s">
         <v>110</v>
       </c>
       <c r="B1" s="4"/>
@@ -10095,19 +10214,19 @@
       <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="80"/>
+      <c r="A2" s="83"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="80"/>
+      <c r="A3" s="83"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="80"/>
+      <c r="A4" s="83"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -10136,7 +10255,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="28">
         <v>2</v>
@@ -10145,7 +10264,7 @@
         <v>56</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="77.25" x14ac:dyDescent="0.25">
@@ -10159,18 +10278,18 @@
         <v>187</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B9" s="28">
         <v>4</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D9" s="60" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="166.5" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="171" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="28">
         <v>5</v>
       </c>
@@ -10178,7 +10297,7 @@
         <v>59</v>
       </c>
       <c r="D10" s="60" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="140.25" x14ac:dyDescent="0.25">
@@ -10189,26 +10308,26 @@
         <v>60</v>
       </c>
       <c r="D11" s="32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="81">
+      <c r="B12" s="80">
         <v>7</v>
       </c>
-      <c r="C12" s="82" t="s">
+      <c r="C12" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="83"/>
+      <c r="D12" s="82"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="81">
+      <c r="B13" s="80">
         <v>8</v>
       </c>
-      <c r="C13" s="82" t="s">
+      <c r="C13" s="81" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="83"/>
+      <c r="D13" s="82"/>
     </row>
     <row r="14" spans="1:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B14" s="28">
@@ -10218,7 +10337,7 @@
         <v>67</v>
       </c>
       <c r="D14" s="60" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -10238,7 +10357,7 @@
         <v>87</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="409.6" x14ac:dyDescent="0.25">

</xml_diff>